<commit_message>
Affichage du score de tous les joueurs en fin de partie
</commit_message>
<xml_diff>
--- a/Burn_Up_Down.xlsx
+++ b/Burn_Up_Down.xlsx
@@ -150,7 +150,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -163,8 +163,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -172,14 +178,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
@@ -344,22 +366,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>65</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>82</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>86</c:v>
+                  <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>86</c:v>
+                  <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>86</c:v>
+                  <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>86</c:v>
+                  <c:v>88</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -404,6 +426,22 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:name>Courbe de tendance</c:name>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:intercept val="0"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:cat>
             <c:strRef>
               <c:f>Feuil1!$K$7:$K$12</c:f>
@@ -444,6 +482,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>77</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -460,11 +501,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="321245104"/>
-        <c:axId val="321246672"/>
+        <c:axId val="156252072"/>
+        <c:axId val="156254816"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="321245104"/>
+        <c:axId val="156252072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -507,7 +548,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="321246672"/>
+        <c:crossAx val="156254816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -515,7 +556,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="321246672"/>
+        <c:axId val="156254816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -566,7 +607,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="321245104"/>
+        <c:crossAx val="156252072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1488,10 +1529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B6:M38"/>
+  <dimension ref="B6:M42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1557,11 +1598,11 @@
         <v>33</v>
       </c>
       <c r="L7">
-        <f>SUM(C$7:C$36)-C29-C30-C32-C33-C35-C36</f>
-        <v>65</v>
+        <f>SUM(C$7:C$34)-C37-C38-C39-C40-C33-C34</f>
+        <v>54</v>
       </c>
       <c r="M7">
-        <f>SUM(D7:D36)</f>
+        <f>SUM(D7:D34)</f>
         <v>17</v>
       </c>
     </row>
@@ -1592,11 +1633,11 @@
         <v>34</v>
       </c>
       <c r="L8">
-        <f>SUM(C$7:C$36)-4</f>
-        <v>82</v>
+        <f>SUM(C$7:C$34)-4</f>
+        <v>73</v>
       </c>
       <c r="M8">
-        <f>SUM(E7:E37)</f>
+        <f>SUM(E7:E41)</f>
         <v>34</v>
       </c>
     </row>
@@ -1627,11 +1668,11 @@
         <v>35</v>
       </c>
       <c r="L9">
-        <f t="shared" ref="L8:L12" si="2">SUM(C$7:C$36)</f>
-        <v>86</v>
+        <f>SUM(C$7:C$40)</f>
+        <v>88</v>
       </c>
       <c r="M9">
-        <f>SUM(F7:F37)</f>
+        <f>SUM(F7:F41)</f>
         <v>58</v>
       </c>
     </row>
@@ -1662,8 +1703,12 @@
         <v>36</v>
       </c>
       <c r="L10">
-        <f t="shared" si="2"/>
-        <v>86</v>
+        <f t="shared" ref="L10:L12" si="2">SUM(C$7:C$40)</f>
+        <v>88</v>
+      </c>
+      <c r="M10">
+        <f>SUM(G7:G34)</f>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
@@ -1694,7 +1739,7 @@
       </c>
       <c r="L11">
         <f t="shared" si="2"/>
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
@@ -1703,7 +1748,7 @@
       </c>
       <c r="L12">
         <f t="shared" si="2"/>
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
@@ -1834,11 +1879,11 @@
         <v>4</v>
       </c>
       <c r="F23">
-        <f>$C23</f>
+        <f t="shared" ref="F23:G26" si="5">$C23</f>
         <v>4</v>
       </c>
       <c r="G23">
-        <f>$C23</f>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
     </row>
@@ -1850,11 +1895,11 @@
         <v>8</v>
       </c>
       <c r="F24">
-        <f>$C24</f>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="G24">
-        <f>$C24</f>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
     </row>
@@ -1866,11 +1911,11 @@
         <v>8</v>
       </c>
       <c r="F25">
-        <f>$C25</f>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="G25">
-        <f>$C25</f>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
     </row>
@@ -1882,28 +1927,12 @@
         <v>4</v>
       </c>
       <c r="F26">
-        <f>$C26</f>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="G26">
-        <f>$C26</f>
+        <f t="shared" si="5"/>
         <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C29">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C30">
-        <v>2</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
@@ -1913,70 +1942,104 @@
       <c r="C31">
         <v>3</v>
       </c>
+      <c r="G31">
+        <v>3</v>
+      </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B32" s="1" t="s">
-        <v>25</v>
+      <c r="B32" t="s">
+        <v>27</v>
       </c>
       <c r="C32">
         <v>4</v>
       </c>
+      <c r="G32">
+        <v>4</v>
+      </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33">
+        <v>6</v>
+      </c>
+      <c r="G33">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C34">
+        <v>6</v>
+      </c>
+      <c r="G34">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35" s="3"/>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B36" s="3"/>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B37" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B38" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B39" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C39">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B40" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C33">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>27</v>
-      </c>
-      <c r="C34">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C35">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B36" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C36">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
+      <c r="C40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
         <v>31</v>
       </c>
-      <c r="C38">
-        <f>SUM(C7:C36)</f>
-        <v>86</v>
-      </c>
-      <c r="D38">
-        <f t="shared" ref="D38:G38" si="5">SUM(D7:D36)</f>
+      <c r="C42">
+        <f>SUM(C7:C40)</f>
+        <v>88</v>
+      </c>
+      <c r="D42">
+        <f>SUM(D7:D34)</f>
         <v>17</v>
       </c>
-      <c r="E38">
-        <f t="shared" si="5"/>
+      <c r="E42">
+        <f>SUM(E7:E34)</f>
         <v>34</v>
       </c>
-      <c r="F38">
-        <f t="shared" si="5"/>
+      <c r="F42">
+        <f>SUM(F7:F34)</f>
         <v>58</v>
       </c>
-      <c r="G38">
-        <f t="shared" si="5"/>
-        <v>58</v>
+      <c r="G42">
+        <f>SUM(G7:G34)</f>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changement de la première pièce (numero 12 pour tous)
</commit_message>
<xml_diff>
--- a/Burn_Up_Down.xlsx
+++ b/Burn_Up_Down.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Total Carte</t>
   </si>
@@ -133,9 +133,6 @@
   </si>
   <si>
     <t>Sprint 5</t>
-  </si>
-  <si>
-    <t>Sprint 6</t>
   </si>
 </sst>
 </file>
@@ -150,7 +147,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -166,6 +163,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -200,8 +203,8 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
@@ -291,7 +294,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="4.1523701642255981E-2"/>
+          <c:y val="9.401774397972118E-2"/>
+          <c:w val="0.94246597290117751"/>
+          <c:h val="0.78919293833517956"/>
+        </c:manualLayout>
+      </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
@@ -335,9 +348,16 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Feuil1!$K$7:$K$12</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Feuil1!$K$7:$K$12</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Feuil1!$K$7:$K$11</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>Sprint 1</c:v>
                 </c:pt>
@@ -353,18 +373,22 @@
                 <c:pt idx="4">
                   <c:v>Sprint 5</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>Sprint 6</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$L$7:$L$12</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Feuil1!$L$7:$L$12</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Feuil1!$L$7:$L$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>54</c:v>
                 </c:pt>
@@ -378,9 +402,6 @@
                   <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>88</c:v>
-                </c:pt>
-                <c:pt idx="5">
                   <c:v>88</c:v>
                 </c:pt>
               </c:numCache>
@@ -444,9 +465,16 @@
           </c:trendline>
           <c:cat>
             <c:strRef>
-              <c:f>Feuil1!$K$7:$K$12</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Feuil1!$K$7:$K$12</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Feuil1!$K$7:$K$11</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>Sprint 1</c:v>
                 </c:pt>
@@ -462,18 +490,22 @@
                 <c:pt idx="4">
                   <c:v>Sprint 5</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>Sprint 6</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$M$7:$M$12</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Feuil1!$M$7:$M$12</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Feuil1!$M$7:$M$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>17</c:v>
                 </c:pt>
@@ -501,11 +533,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="156252072"/>
-        <c:axId val="156254816"/>
+        <c:axId val="151722032"/>
+        <c:axId val="151722424"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="156252072"/>
+        <c:axId val="151722032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -548,7 +580,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="156254816"/>
+        <c:crossAx val="151722424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -556,7 +588,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="156254816"/>
+        <c:axId val="151722424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -607,7 +639,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="156252072"/>
+        <c:crossAx val="151722032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1235,16 +1267,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>114299</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>46905</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>180974</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>147637</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>390524</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1529,10 +1561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B6:M42"/>
+  <dimension ref="B6:N42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1542,7 +1574,7 @@
     <col min="8" max="9" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>8</v>
       </c>
@@ -1571,7 +1603,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>9</v>
       </c>
@@ -1605,8 +1637,12 @@
         <f>SUM(D7:D34)</f>
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="N7">
+        <f>M8-M7</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>13</v>
       </c>
@@ -1640,8 +1676,12 @@
         <f>SUM(E7:E41)</f>
         <v>34</v>
       </c>
-    </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="N8">
+        <f t="shared" ref="N8:N9" si="2">M9-M8</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>17</v>
       </c>
@@ -1675,9 +1715,13 @@
         <f>SUM(F7:F41)</f>
         <v>58</v>
       </c>
-    </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+      <c r="N9">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C10">
@@ -1703,7 +1747,7 @@
         <v>36</v>
       </c>
       <c r="L10">
-        <f t="shared" ref="L10:L12" si="2">SUM(C$7:C$40)</f>
+        <f t="shared" ref="L10:L12" si="3">SUM(C$7:C$40)</f>
         <v>88</v>
       </c>
       <c r="M10">
@@ -1711,7 +1755,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>20</v>
       </c>
@@ -1738,20 +1782,11 @@
         <v>37</v>
       </c>
       <c r="L11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>88</v>
       </c>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="K12" t="s">
-        <v>38</v>
-      </c>
-      <c r="L12">
-        <f t="shared" si="2"/>
-        <v>88</v>
-      </c>
-    </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>11</v>
       </c>
@@ -1763,15 +1798,15 @@
         <v>4</v>
       </c>
       <c r="F14">
-        <f t="shared" ref="F14:G19" si="3">$C14</f>
+        <f t="shared" ref="F14:G19" si="4">$C14</f>
         <v>4</v>
       </c>
       <c r="G14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>10</v>
       </c>
@@ -1779,19 +1814,19 @@
         <v>2</v>
       </c>
       <c r="E15">
-        <f t="shared" ref="E15:E19" si="4">$C15</f>
+        <f t="shared" ref="E15:E19" si="5">$C15</f>
         <v>2</v>
       </c>
       <c r="F15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="G15">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>12</v>
       </c>
@@ -1799,15 +1834,15 @@
         <v>2</v>
       </c>
       <c r="E16">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="F16">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="F16">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
       <c r="G16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
     </row>
@@ -1819,35 +1854,35 @@
         <v>2</v>
       </c>
       <c r="E17">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="F17">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="F17">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
       <c r="G17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+      <c r="B18" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C18">
         <v>5</v>
       </c>
       <c r="E18">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="F18">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="F18">
-        <f t="shared" si="3"/>
-        <v>5</v>
-      </c>
       <c r="G18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
@@ -1859,15 +1894,15 @@
         <v>2</v>
       </c>
       <c r="E19">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="F19">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="F19">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
       <c r="G19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
     </row>
@@ -1879,43 +1914,43 @@
         <v>4</v>
       </c>
       <c r="F23">
-        <f t="shared" ref="F23:G26" si="5">$C23</f>
+        <f t="shared" ref="F23:G26" si="6">$C23</f>
         <v>4</v>
       </c>
       <c r="G23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
+      <c r="B24" s="3" t="s">
         <v>28</v>
       </c>
       <c r="C24">
         <v>8</v>
       </c>
       <c r="F24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="G24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
+      <c r="B25" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C25">
         <v>8</v>
       </c>
       <c r="F25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="G25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
     </row>
@@ -1927,16 +1962,16 @@
         <v>4</v>
       </c>
       <c r="F26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="G26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="3" t="s">
         <v>24</v>
       </c>
       <c r="C31">
@@ -1947,7 +1982,7 @@
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
+      <c r="B32" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C32">
@@ -1958,7 +1993,7 @@
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="1" t="s">
+      <c r="B33" s="3" t="s">
         <v>29</v>
       </c>
       <c r="C33">
@@ -1980,10 +2015,10 @@
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="3"/>
+      <c r="B35" s="2"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B36" s="3"/>
+      <c r="B36" s="2"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">

</xml_diff>

<commit_message>
Burn Up sprint 8
</commit_message>
<xml_diff>
--- a/Burn_Up_Down.xlsx
+++ b/Burn_Up_Down.xlsx
@@ -5,32 +5,23 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projets\blokus\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Documents\Cours\IUT\S3\Blokus\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10875"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10872"/>
   </bookViews>
   <sheets>
     <sheet name="Itérations" sheetId="1" r:id="rId1"/>
     <sheet name="Sprint 7" sheetId="2" r:id="rId2"/>
+    <sheet name="Sprint 8" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'Sprint 7'!$B$1</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'Sprint 7'!$B$2:$B$8</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'Sprint 7'!$C$1</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'Sprint 7'!$C$2:$C$8</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'Sprint 7'!$B$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'Sprint 7'!$B$4:$B$12</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">'Sprint 7'!$C$1</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">'Sprint 7'!$C$4:$C$12</definedName>
-  </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="80">
   <si>
     <t>Total Carte</t>
   </si>
@@ -158,9 +149,6 @@
     <t>sous total Relase 2</t>
   </si>
   <si>
-    <t>Serveur pour chaque partie de X personnes selon le mode de jeu</t>
-  </si>
-  <si>
     <t>Recevoir envoyer les données (serveur</t>
   </si>
   <si>
@@ -243,6 +231,36 @@
   </si>
   <si>
     <t>Nan</t>
+  </si>
+  <si>
+    <t>IA</t>
+  </si>
+  <si>
+    <t>Serveur de jeu (Gestion des requetes)</t>
+  </si>
+  <si>
+    <t>Serveur de jeu (Gestion des threads)</t>
+  </si>
+  <si>
+    <t>Nouvelle partie dans menu démarrer</t>
+  </si>
+  <si>
+    <t>Gestion fin de partie (retour à l'accueil)</t>
+  </si>
+  <si>
+    <t>Amélioration Accueil</t>
+  </si>
+  <si>
+    <t>Début du srint</t>
+  </si>
+  <si>
+    <t>Amélioration Acceuil</t>
+  </si>
+  <si>
+    <t>Serveur pour chaque partie de X personnes</t>
+  </si>
+  <si>
+    <t>Point de release</t>
   </si>
 </sst>
 </file>
@@ -380,7 +398,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -515,16 +532,16 @@
                   <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>199</c:v>
+                  <c:v>202</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>199</c:v>
+                  <c:v>202</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>199</c:v>
+                  <c:v>202</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>199</c:v>
+                  <c:v>202</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -644,6 +661,9 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>148</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -784,7 +804,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -891,7 +910,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1236,6 +1254,378 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>BurnDown Sprint 8</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint 8'!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Sprint 8'!$E$2:$E$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Sprint 8'!$F$2:$F$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A46F-4CA3-BBC9-7D70EE01C7E3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="328615760"/>
+        <c:axId val="328610840"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="328615760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="328610840"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="328610840"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="328615760"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1316,6 +1706,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="342">
   <cs:axisTitle>
@@ -1819,6 +2249,508 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="343">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="343">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2373,6 +3305,41 @@
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="4" name="Graphique 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>182880</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Graphique 4"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2466,6 +3433,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2501,6 +3485,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2653,20 +3654,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B6:M78"/>
+  <dimension ref="B6:Q77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="E6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
-    <col min="2" max="2" width="30.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.44140625" customWidth="1"/>
+    <col min="2" max="2" width="30.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>8</v>
       </c>
@@ -2694,8 +3696,11 @@
       <c r="M6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="Q6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>9</v>
       </c>
@@ -2729,8 +3734,12 @@
         <f>SUM(D7:D34)</f>
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="Q7">
+        <f>SUM(C42:C67)</f>
+        <v>188</v>
+      </c>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>13</v>
       </c>
@@ -2765,7 +3774,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>17</v>
       </c>
@@ -2800,7 +3809,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B10" s="3" t="s">
         <v>18</v>
       </c>
@@ -2835,7 +3844,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>20</v>
       </c>
@@ -2870,33 +3879,33 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:17" x14ac:dyDescent="0.3">
       <c r="K12" t="s">
         <v>37</v>
       </c>
       <c r="L12">
-        <f>C78</f>
-        <v>199</v>
+        <f>C77</f>
+        <v>202</v>
       </c>
       <c r="M12">
-        <f>D75</f>
+        <f>D74</f>
         <v>96</v>
       </c>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:17" x14ac:dyDescent="0.3">
       <c r="K13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L13">
-        <f>C78</f>
-        <v>199</v>
+        <f>C77</f>
+        <v>202</v>
       </c>
       <c r="M13">
-        <f>E75</f>
+        <f>E74</f>
         <v>121</v>
       </c>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>11</v>
       </c>
@@ -2916,14 +3925,18 @@
         <v>4</v>
       </c>
       <c r="K14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L14">
-        <f>C78</f>
-        <v>199</v>
-      </c>
-    </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+        <f>C77</f>
+        <v>202</v>
+      </c>
+      <c r="M14">
+        <f>F74</f>
+        <v>148</v>
+      </c>
+    </row>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>10</v>
       </c>
@@ -2943,14 +3956,14 @@
         <v>2</v>
       </c>
       <c r="K15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L15">
-        <f>C78</f>
-        <v>199</v>
-      </c>
-    </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+        <f>C77</f>
+        <v>202</v>
+      </c>
+    </row>
+    <row r="16" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>12</v>
       </c>
@@ -2970,7 +3983,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>14</v>
       </c>
@@ -2990,7 +4003,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B18" s="3" t="s">
         <v>19</v>
       </c>
@@ -3010,7 +4023,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>21</v>
       </c>
@@ -3030,7 +4043,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>16</v>
       </c>
@@ -3046,7 +4059,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B24" s="3" t="s">
         <v>28</v>
       </c>
@@ -3062,7 +4075,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B25" s="3" t="s">
         <v>22</v>
       </c>
@@ -3078,7 +4091,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>23</v>
       </c>
@@ -3094,7 +4107,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B31" s="3" t="s">
         <v>24</v>
       </c>
@@ -3105,7 +4118,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B32" s="3" t="s">
         <v>27</v>
       </c>
@@ -3116,7 +4129,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B33" s="3" t="s">
         <v>29</v>
       </c>
@@ -3127,7 +4140,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B34" s="1" t="s">
         <v>30</v>
       </c>
@@ -3138,13 +4151,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B35" s="2"/>
     </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B36" s="2"/>
     </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B37" s="1" t="s">
         <v>31</v>
       </c>
@@ -3152,7 +4165,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B38" s="1" t="s">
         <v>15</v>
       </c>
@@ -3160,7 +4173,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B39" s="1" t="s">
         <v>25</v>
       </c>
@@ -3168,7 +4181,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B40" s="1" t="s">
         <v>26</v>
       </c>
@@ -3176,7 +4189,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
         <v>40</v>
       </c>
@@ -3201,7 +4214,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
         <v>38</v>
       </c>
@@ -3224,7 +4237,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
         <v>39</v>
       </c>
@@ -3239,7 +4252,7 @@
         <v>2</v>
       </c>
       <c r="F46">
-        <f t="shared" ref="F46:G46" si="6">D46</f>
+        <f t="shared" ref="F46:H46" si="6">D46</f>
         <v>2</v>
       </c>
       <c r="G46">
@@ -3247,9 +4260,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B49" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C49">
         <v>6</v>
@@ -3263,13 +4276,13 @@
         <v>6</v>
       </c>
       <c r="G49">
-        <f t="shared" ref="F49:G54" si="7">E49</f>
+        <f t="shared" ref="G49:H54" si="7">E49</f>
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B50" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C50">
         <v>4</v>
@@ -3287,9 +4300,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B51" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C51">
         <v>2</v>
@@ -3307,9 +4320,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B52" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C52">
         <v>3</v>
@@ -3327,9 +4340,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B53" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C53">
         <v>5</v>
@@ -3347,9 +4360,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B54" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C54">
         <v>5</v>
@@ -3367,155 +4380,170 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B55" s="4"/>
     </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B56" s="4"/>
     </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B57" s="4"/>
-    </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B57" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C57">
+        <v>10</v>
+      </c>
+      <c r="F57">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B58" s="4" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="C58">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B59" s="4"/>
-    </row>
-    <row r="60" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B60" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C60">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="61" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="F58">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B59" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C59">
+        <v>7</v>
+      </c>
+      <c r="F59">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B61" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C61">
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B62" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C62">
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B63" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C63">
         <v>8</v>
       </c>
     </row>
-    <row r="64" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B64" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C64">
         <v>8</v>
       </c>
     </row>
-    <row r="65" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B65" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C65">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B66" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C66">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B67" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C67">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B69" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C69">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="70" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B70" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C70">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="71" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B71" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C71">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B72" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C65">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B66" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C66">
+      <c r="C72">
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B67" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C67">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B68" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C68">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B69" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C69">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B70" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C70">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B73" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C73">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="75" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B75" t="s">
+    <row r="74" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B74" t="s">
         <v>41</v>
       </c>
-      <c r="C75">
-        <f>SUM(C42:C73)</f>
-        <v>231</v>
-      </c>
-      <c r="D75">
+      <c r="C74">
+        <f>SUM(C42:C67)</f>
+        <v>188</v>
+      </c>
+      <c r="D74">
         <f>SUM(D45:D46,C42)</f>
         <v>96</v>
       </c>
-      <c r="E75">
+      <c r="E74">
         <f>SUM(E45:E54,C42)</f>
         <v>121</v>
       </c>
-    </row>
-    <row r="77" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F74">
+        <f>SUM(F45:F67,C42)</f>
+        <v>148</v>
+      </c>
+    </row>
+    <row r="76" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B76" t="s">
+        <v>63</v>
+      </c>
+      <c r="C76">
+        <f>C74</f>
+        <v>188</v>
+      </c>
+    </row>
+    <row r="77" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B77" t="s">
         <v>64</v>
       </c>
       <c r="C77">
-        <f>C75</f>
-        <v>231</v>
-      </c>
-    </row>
-    <row r="78" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B78" t="s">
-        <v>65</v>
-      </c>
-      <c r="C78">
-        <f>SUM(C42:C69)</f>
-        <v>199</v>
+        <f>SUM(C42:C70)</f>
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -3535,35 +4563,35 @@
   <dimension ref="A1:F74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" customWidth="1"/>
-    <col min="3" max="4" width="14.5703125" customWidth="1"/>
+    <col min="1" max="1" width="22.5546875" customWidth="1"/>
+    <col min="3" max="4" width="14.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" t="s">
         <v>66</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>67</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>68</v>
-      </c>
-      <c r="E1" t="s">
-        <v>69</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -3582,9 +4610,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -3602,9 +4630,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B4">
         <v>6</v>
@@ -3623,9 +4651,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -3643,9 +4671,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -3663,9 +4691,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B7">
         <v>5</v>
@@ -3684,23 +4712,23 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B10">
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
     </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B74" s="5"/>
     </row>
   </sheetData>
@@ -3708,4 +4736,176 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="6">
+        <f>DATE(2016,2,12)</f>
+        <v>42412</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <f>SUM(B3:B12)</f>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3" s="6">
+        <f>DATE(2016,3,3)</f>
+        <v>42432</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="7">
+        <v>20</v>
+      </c>
+      <c r="F3">
+        <f>F2-B3-B4</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="C4" s="6">
+        <f>DATE(2016,3,3)</f>
+        <v>42432</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="7">
+        <v>20</v>
+      </c>
+      <c r="F4">
+        <f>F3</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5">
+        <v>7</v>
+      </c>
+      <c r="C5" s="6">
+        <f>DATE(2016,3,4)</f>
+        <v>42433</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="7">
+        <v>21</v>
+      </c>
+      <c r="F5">
+        <f>F4-B5</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="4"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="7"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="4"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="7"/>
+    </row>
+    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="7"/>
+    </row>
+    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="7"/>
+    </row>
+    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" s="6"/>
+      <c r="E10" s="7"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="4"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="4"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>